<commit_message>
Evaluations: #35, updated graphics for document accesses
</commit_message>
<xml_diff>
--- a/eval/e35/doc_accesses.xlsx
+++ b/eval/e35/doc_accesses.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -48,41 +48,41 @@
     <t>P8</t>
   </si>
   <si>
-    <t>CSS1</t>
-  </si>
-  <si>
-    <t>CSS2</t>
-  </si>
-  <si>
-    <t>CSS3</t>
-  </si>
-  <si>
-    <t>CSS4</t>
-  </si>
-  <si>
-    <t>wget1</t>
-  </si>
-  <si>
-    <t>wget2</t>
-  </si>
-  <si>
-    <t>wget3</t>
-  </si>
-  <si>
-    <t>wget4</t>
-  </si>
-  <si>
     <t>Task</t>
   </si>
   <si>
     <t>D</t>
+  </si>
+  <si>
+    <t>CSS 1</t>
+  </si>
+  <si>
+    <t>CSS 2</t>
+  </si>
+  <si>
+    <t>CSS 3</t>
+  </si>
+  <si>
+    <t>CSS 4</t>
+  </si>
+  <si>
+    <t>wget 1</t>
+  </si>
+  <si>
+    <t>wget 2</t>
+  </si>
+  <si>
+    <t>wget 3</t>
+  </si>
+  <si>
+    <t>wget 4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="16"/>
       <color theme="1"/>
@@ -120,12 +120,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="16"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -133,17 +127,28 @@
     </font>
     <font>
       <sz val="16"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
+      <sz val="16"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <name val="Helvetica"/>
     </font>
     <font>
       <b/>
       <sz val="16"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
+      <name val="Helvetica"/>
     </font>
   </fonts>
   <fills count="4">
@@ -312,7 +317,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -323,59 +328,83 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="41">
@@ -754,287 +783,287 @@
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="6.88671875" customWidth="1"/>
-    <col min="2" max="6" width="4.44140625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="5" style="2" customWidth="1"/>
-    <col min="8" max="8" width="6.44140625" style="2" customWidth="1"/>
-    <col min="9" max="11" width="4.44140625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="5.21875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="7.109375" style="28" customWidth="1"/>
+    <col min="2" max="6" width="4.33203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="3.6640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="7.109375" style="28" customWidth="1"/>
+    <col min="9" max="12" width="4.33203125" style="2" customWidth="1"/>
     <col min="13" max="13" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
-      <c r="A1" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:13" s="2" customFormat="1" ht="22" customHeight="1">
+      <c r="A1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I1" s="2" t="s">
+      <c r="G1" s="8"/>
+      <c r="H1" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="8" t="s">
         <v>8</v>
       </c>
       <c r="M1" s="3"/>
     </row>
-    <row r="2" spans="1:13">
-      <c r="A2" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="5"/>
+    <row r="2" spans="1:13" s="2" customFormat="1" ht="22" customHeight="1">
+      <c r="A2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="4"/>
     </row>
-    <row r="3" spans="1:13">
-      <c r="A3" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="18" t="s">
+    <row r="3" spans="1:13" s="2" customFormat="1" ht="22" customHeight="1">
+      <c r="A3" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="17"/>
+      <c r="H3" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="4"/>
+    </row>
+    <row r="4" spans="1:13" s="2" customFormat="1" ht="22" customHeight="1">
+      <c r="A4" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="M4" s="4"/>
+    </row>
+    <row r="5" spans="1:13" s="2" customFormat="1" ht="22" customHeight="1">
+      <c r="A5" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="14"/>
+      <c r="C5" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="17"/>
+      <c r="H5" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="4"/>
+    </row>
+    <row r="6" spans="1:13" s="5" customFormat="1" ht="22" customHeight="1">
+      <c r="A6" s="21"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="22"/>
+      <c r="M6" s="4"/>
+    </row>
+    <row r="7" spans="1:13" s="2" customFormat="1" ht="22" customHeight="1">
+      <c r="A7" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="K7" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="L7" s="14"/>
+      <c r="M7" s="4"/>
+    </row>
+    <row r="8" spans="1:13" s="2" customFormat="1" ht="22" customHeight="1">
+      <c r="A8" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="14"/>
+      <c r="E8" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="17"/>
+      <c r="H8" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="4"/>
+    </row>
+    <row r="9" spans="1:13" s="2" customFormat="1" ht="22" customHeight="1">
+      <c r="A9" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="J9" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="K9" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="L9" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="M9" s="4"/>
+    </row>
+    <row r="10" spans="1:13" s="2" customFormat="1" ht="22" customHeight="1">
+      <c r="A10" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="B10" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="17"/>
+      <c r="H10" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="8"/>
-      <c r="H3" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="5"/>
-    </row>
-    <row r="4" spans="1:13">
-      <c r="A4" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="M4" s="5"/>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="A5" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="17"/>
-      <c r="C5" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="8"/>
-      <c r="H5" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
-      <c r="M5" s="5"/>
-    </row>
-    <row r="6" spans="1:13" s="16" customFormat="1">
-      <c r="A6" s="13"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="5"/>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="A7" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="I7" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="J7" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="K7" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="L7" s="17"/>
-      <c r="M7" s="5"/>
-    </row>
-    <row r="8" spans="1:13">
-      <c r="A8" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="17"/>
-      <c r="E8" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" s="8"/>
-      <c r="H8" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="20"/>
-      <c r="M8" s="5"/>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="A9" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="I9" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="J9" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="K9" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="L9" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="M9" s="5"/>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="A10" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="G10" s="8"/>
-      <c r="H10" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="I10" s="20"/>
-      <c r="J10" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="K10" s="20"/>
-      <c r="L10" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="M10" s="5"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="K10" s="19"/>
+      <c r="L10" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="M10" s="4"/>
     </row>
     <row r="11" spans="1:13">
-      <c r="A11" s="4"/>
+      <c r="A11" s="29"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
+      <c r="H11" s="27"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="10"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="6"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="93" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup scale="96" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="100"/>

</xml_diff>